<commit_message>
Modifications in year used for the calculation
</commit_message>
<xml_diff>
--- a/prep/CW/cw_trash_trend_mse2019.xlsx
+++ b/prep/CW/cw_trash_trend_mse2019.xlsx
@@ -1,27 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\AGUAS LIMPIAS\CAPAS DE DATOS AGUAS LIMPIAS\EXCELS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Hurtadoyhurtado\carpeta compartida\PROYECTOS\CI IdSO MANABÍ Y SANTA ELENA\CAPAS DE DATOS\DATOS CRUDOS\AGUAS LIMPIAS\AGUAS LIMPIAS 2019\DATOS CRUDOS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C056DDA-8119-4CCD-BC4E-353DE1268553}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6255" yWindow="4260" windowWidth="8910" windowHeight="7260" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14160" windowHeight="10560"/>
   </bookViews>
   <sheets>
     <sheet name="trash 2010" sheetId="1" r:id="rId1"/>
-    <sheet name="trash 2020" sheetId="2" r:id="rId2"/>
-    <sheet name="calculo trash" sheetId="3" r:id="rId3"/>
-    <sheet name="cw_trash_trend" sheetId="4" r:id="rId4"/>
+    <sheet name="trash 2025" sheetId="2" r:id="rId2"/>
+    <sheet name="PARÁMETROS" sheetId="5" r:id="rId3"/>
+    <sheet name="calculo trash" sheetId="3" r:id="rId4"/>
+    <sheet name="cw_trash_trend" sheetId="4" r:id="rId5"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId5"/>
+    <externalReference r:id="rId6"/>
   </externalReferences>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,31 +37,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="61">
   <si>
     <t>PROVINCIA</t>
   </si>
   <si>
     <t>CANTÓN</t>
-  </si>
-  <si>
-    <t>Coastal population (2010)</t>
-  </si>
-  <si>
-    <r>
-      <t>Waste generation rate [kg/person/day]</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <vertAlign val="superscript"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>3</t>
-    </r>
   </si>
   <si>
     <r>
@@ -338,9 +319,6 @@
     <t>trend10year/10</t>
   </si>
   <si>
-    <t>Projection Coastal population (2020)</t>
-  </si>
-  <si>
     <t>rgn_id</t>
   </si>
   <si>
@@ -349,11 +327,38 @@
   <si>
     <t>trend</t>
   </si>
+  <si>
+    <t>Metodología:  Jambeck et al. (2016). Plastic waste inputs from land into the ocean.</t>
+  </si>
+  <si>
+    <t>Coastal population (2010) [1]</t>
+  </si>
+  <si>
+    <t>Waste generation rate [kg/person/day] [2]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[1] INEC (2019). Censo de Población y Vivienda 2010. http://www.ecuadorencifras.gob.ec/base-de-datos-censo-de-poblacion-y-vivienda/ </t>
+  </si>
+  <si>
+    <t>Metodología:  Jambeck et al. (2016). Plastic waste inputs from land into the ocean. https://science.sciencemag.org/content/suppl/2015/02/11/347.6223.768.DC1</t>
+  </si>
+  <si>
+    <t>[2] MAE (2013). Programa Nacional para la gestión integral de desechos sólidos</t>
+  </si>
+  <si>
+    <t>[2] MAE (2013). Programa Nacional para la gestión integral de desechos sólidos. https://slideplayer.es/slide/3832641/</t>
+  </si>
+  <si>
+    <t>Coastal population (2025) [3]</t>
+  </si>
+  <si>
+    <t>[3] Instituto Nacional de Estadística y Censos (INEC) - Consultora Biótica</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="#,##0.000"/>
@@ -513,7 +518,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="166" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -576,15 +581,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Millares 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="Millares 2" xfId="2"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Porcentaje" xfId="1" builtinId="5"/>
   </cellStyles>
@@ -601,7 +610,3066 @@
 </styleSheet>
 </file>
 
+<file path=xl/diagrams/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<dgm:colorsDef xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uniqueId="urn:microsoft.com/office/officeart/2005/8/colors/accent1_2">
+  <dgm:title val=""/>
+  <dgm:desc val=""/>
+  <dgm:catLst>
+    <dgm:cat type="accent1" pri="11200"/>
+  </dgm:catLst>
+  <dgm:styleLbl name="node0">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="lt1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst/>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="alignNode1">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst/>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="node1">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="lt1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst/>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="lnNode1">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="lt1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst/>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="vennNode1">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1">
+        <a:alpha val="50000"/>
+      </a:schemeClr>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="lt1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst/>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="node2">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="lt1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst/>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="node3">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="lt1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst/>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="node4">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="lt1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst/>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="fgImgPlace1">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1">
+        <a:tint val="50000"/>
+      </a:schemeClr>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="lt1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="lt1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="alignImgPlace1">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1">
+        <a:tint val="50000"/>
+      </a:schemeClr>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="lt1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="lt1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="bgImgPlace1">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1">
+        <a:tint val="50000"/>
+      </a:schemeClr>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="lt1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="lt1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="sibTrans2D1">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1">
+        <a:tint val="60000"/>
+      </a:schemeClr>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1">
+        <a:tint val="60000"/>
+      </a:schemeClr>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst/>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="fgSibTrans2D1">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1">
+        <a:tint val="60000"/>
+      </a:schemeClr>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1">
+        <a:tint val="60000"/>
+      </a:schemeClr>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst/>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="bgSibTrans2D1">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1">
+        <a:tint val="60000"/>
+      </a:schemeClr>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1">
+        <a:tint val="60000"/>
+      </a:schemeClr>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst/>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="sibTrans1D1">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="tx1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="callout">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1">
+        <a:tint val="50000"/>
+      </a:schemeClr>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="tx1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="asst0">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="lt1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst/>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="asst1">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="lt1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst/>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="asst2">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="lt1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst/>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="asst3">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="lt1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst/>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="asst4">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="lt1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst/>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="parChTrans2D1">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1">
+        <a:tint val="60000"/>
+      </a:schemeClr>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1">
+        <a:tint val="60000"/>
+      </a:schemeClr>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="lt1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="parChTrans2D2">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="lt1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="parChTrans2D3">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="lt1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="parChTrans2D4">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="lt1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="parChTrans1D1">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1">
+        <a:shade val="60000"/>
+      </a:schemeClr>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="tx1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="parChTrans1D2">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1">
+        <a:shade val="60000"/>
+      </a:schemeClr>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="tx1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="parChTrans1D3">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1">
+        <a:shade val="80000"/>
+      </a:schemeClr>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="tx1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="parChTrans1D4">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1">
+        <a:shade val="80000"/>
+      </a:schemeClr>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="tx1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="fgAcc1">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="lt1">
+        <a:alpha val="90000"/>
+      </a:schemeClr>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="dk1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="conFgAcc1">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="lt1">
+        <a:alpha val="90000"/>
+      </a:schemeClr>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="dk1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="alignAcc1">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="lt1">
+        <a:alpha val="90000"/>
+      </a:schemeClr>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="dk1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="trAlignAcc1">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="lt1">
+        <a:alpha val="40000"/>
+      </a:schemeClr>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="dk1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="bgAcc1">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="lt1">
+        <a:alpha val="90000"/>
+      </a:schemeClr>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="dk1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="solidFgAcc1">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="lt1"/>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="dk1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="solidAlignAcc1">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="lt1"/>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="dk1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="solidBgAcc1">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="lt1"/>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="dk1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="fgAccFollowNode1">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1">
+        <a:alpha val="90000"/>
+        <a:tint val="40000"/>
+      </a:schemeClr>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1">
+        <a:alpha val="90000"/>
+        <a:tint val="40000"/>
+      </a:schemeClr>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="dk1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="alignAccFollowNode1">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1">
+        <a:alpha val="90000"/>
+        <a:tint val="40000"/>
+      </a:schemeClr>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1">
+        <a:alpha val="90000"/>
+        <a:tint val="40000"/>
+      </a:schemeClr>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="dk1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="bgAccFollowNode1">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1">
+        <a:alpha val="90000"/>
+        <a:tint val="40000"/>
+      </a:schemeClr>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1">
+        <a:alpha val="90000"/>
+        <a:tint val="40000"/>
+      </a:schemeClr>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="dk1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="fgAcc0">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="lt1">
+        <a:alpha val="90000"/>
+      </a:schemeClr>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="dk1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="fgAcc2">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="lt1">
+        <a:alpha val="90000"/>
+      </a:schemeClr>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="dk1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="fgAcc3">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="lt1">
+        <a:alpha val="90000"/>
+      </a:schemeClr>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="dk1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="fgAcc4">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="lt1">
+        <a:alpha val="90000"/>
+      </a:schemeClr>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="dk1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="bgShp">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1">
+        <a:tint val="40000"/>
+      </a:schemeClr>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="dk1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="dkBgShp">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1">
+        <a:shade val="80000"/>
+      </a:schemeClr>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="lt1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="trBgShp">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1">
+        <a:tint val="50000"/>
+        <a:alpha val="40000"/>
+      </a:schemeClr>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="lt1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="fgShp">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1">
+        <a:tint val="60000"/>
+      </a:schemeClr>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="lt1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="dk1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="revTx">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="lt1">
+        <a:alpha val="0"/>
+      </a:schemeClr>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="dk1">
+        <a:alpha val="0"/>
+      </a:schemeClr>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="tx1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+</dgm:colorsDef>
+</file>
+
+<file path=xl/diagrams/data1.xml><?xml version="1.0" encoding="utf-8"?>
+<dgm:dataModel xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <dgm:ptLst>
+    <dgm:pt modelId="{3D58A12A-B9B8-264E-BD9E-E85FA3CBA9EA}" type="doc">
+      <dgm:prSet loTypeId="urn:microsoft.com/office/officeart/2005/8/layout/vList5" loCatId="" qsTypeId="urn:microsoft.com/office/officeart/2005/8/quickstyle/simple4" qsCatId="simple" csTypeId="urn:microsoft.com/office/officeart/2005/8/colors/accent1_2" csCatId="accent1" phldr="1"/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{E198C860-F583-3A45-B783-2F1B64498303}">
+      <dgm:prSet phldrT="[Text]" custT="1"/>
+      <dgm:spPr>
+        <a:solidFill>
+          <a:srgbClr val="2B8DD9">
+            <a:alpha val="90000"/>
+          </a:srgbClr>
+        </a:solidFill>
+      </dgm:spPr>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="es-EC" sz="1800" noProof="0" dirty="0"/>
+            <a:t>GAD Grande</a:t>
+          </a:r>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{AEB4A8E4-1F1E-D84E-B712-6CFC524438EE}" type="parTrans" cxnId="{B92E82A1-2AC9-1E46-9B77-DA221A30937C}">
+      <dgm:prSet/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{6EBA461A-EF40-7C42-808C-13AB114788E8}" type="sibTrans" cxnId="{B92E82A1-2AC9-1E46-9B77-DA221A30937C}">
+      <dgm:prSet/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{541570D1-BB87-5142-A402-22840FAA1C66}">
+      <dgm:prSet phldrT="[Text]" custT="1"/>
+      <dgm:spPr>
+        <a:solidFill>
+          <a:srgbClr val="2B8DD9"/>
+        </a:solidFill>
+      </dgm:spPr>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-EC" sz="1400" noProof="0" dirty="0"/>
+            <a:t>PPC: 0.75 kg/</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-EC" sz="1400" noProof="0" dirty="0" err="1"/>
+            <a:t>hab.día</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-EC" sz="1400" noProof="0" dirty="0"/>
+            <a:t> *</a:t>
+          </a:r>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{D899A435-369B-3641-96A7-864ED0FE03AD}" type="parTrans" cxnId="{F8434D64-C311-A743-95CC-1EED8CCDDBF9}">
+      <dgm:prSet/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{17AC0375-E1CE-3940-82EE-7586D4188233}" type="sibTrans" cxnId="{F8434D64-C311-A743-95CC-1EED8CCDDBF9}">
+      <dgm:prSet/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{7A9F7AFA-C04E-BD4D-82F0-C72444B4257E}">
+      <dgm:prSet phldrT="[Text]" custT="1"/>
+      <dgm:spPr>
+        <a:solidFill>
+          <a:srgbClr val="2B8DD9"/>
+        </a:solidFill>
+      </dgm:spPr>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-EC" sz="1400" noProof="0" dirty="0"/>
+            <a:t>Cobertura: 85.29% **</a:t>
+          </a:r>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{6543371B-5BBE-4743-BE56-5A7F7669D274}" type="parTrans" cxnId="{2E0A4BCC-A4B1-7144-B28A-D0A45104CA3B}">
+      <dgm:prSet/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{C427DA95-AF77-2349-8B32-BE493CCB5CE3}" type="sibTrans" cxnId="{2E0A4BCC-A4B1-7144-B28A-D0A45104CA3B}">
+      <dgm:prSet/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{3B22AF23-C402-284E-94ED-F6615174E79D}">
+      <dgm:prSet phldrT="[Text]" custT="1"/>
+      <dgm:spPr>
+        <a:solidFill>
+          <a:srgbClr val="37C9D3">
+            <a:alpha val="90000"/>
+          </a:srgbClr>
+        </a:solidFill>
+      </dgm:spPr>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="es-EC" sz="1800" noProof="0" dirty="0"/>
+            <a:t>GAD Mediano</a:t>
+          </a:r>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{4444906B-EB1F-D14E-AFB8-F39CE987C67F}" type="parTrans" cxnId="{3FA8B827-CE26-AB4E-AFEA-A2D349DC1784}">
+      <dgm:prSet/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{D4B4AB0A-4AB5-034E-AEA2-8BFBB76563F6}" type="sibTrans" cxnId="{3FA8B827-CE26-AB4E-AFEA-A2D349DC1784}">
+      <dgm:prSet/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{4B9D3448-F1F1-A64B-B475-FF5B1414BA51}">
+      <dgm:prSet phldrT="[Text]" custT="1"/>
+      <dgm:spPr>
+        <a:solidFill>
+          <a:srgbClr val="37C9D3"/>
+        </a:solidFill>
+      </dgm:spPr>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-EC" sz="1400" noProof="0" dirty="0"/>
+            <a:t>PPC: 0.68 kg/</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-EC" sz="1400" noProof="0" dirty="0" err="1"/>
+            <a:t>hab.día</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-EC" sz="1400" noProof="0" dirty="0"/>
+            <a:t> *</a:t>
+          </a:r>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{908EBDA6-70C5-B248-A16B-7D0276715C37}" type="parTrans" cxnId="{D4A9EAFB-8EFA-A844-9109-55519A64765F}">
+      <dgm:prSet/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{5C186B2D-E6AB-EF4D-B949-98ED92504A65}" type="sibTrans" cxnId="{D4A9EAFB-8EFA-A844-9109-55519A64765F}">
+      <dgm:prSet/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{ECB1009C-45F1-AD49-8507-8844A4E0AC68}">
+      <dgm:prSet phldrT="[Text]" custT="1"/>
+      <dgm:spPr>
+        <a:solidFill>
+          <a:srgbClr val="15D180">
+            <a:alpha val="90000"/>
+          </a:srgbClr>
+        </a:solidFill>
+      </dgm:spPr>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="es-EC" sz="1800" noProof="0" dirty="0"/>
+            <a:t>GAD Pequeño</a:t>
+          </a:r>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{E14009BB-621C-2A41-A673-C557A1CA377B}" type="parTrans" cxnId="{DF28298D-C9F3-2147-85E8-D39D967E3067}">
+      <dgm:prSet/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{CE595159-41CD-D443-8F5F-79EF4DC30577}" type="sibTrans" cxnId="{DF28298D-C9F3-2147-85E8-D39D967E3067}">
+      <dgm:prSet/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{FC7B3C0A-79EE-C043-98FB-AA5109650539}">
+      <dgm:prSet phldrT="[Text]" custT="1"/>
+      <dgm:spPr>
+        <a:solidFill>
+          <a:srgbClr val="15D180"/>
+        </a:solidFill>
+      </dgm:spPr>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-EC" sz="1400" noProof="0" dirty="0"/>
+            <a:t>PPC: 0.61 kg/</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-EC" sz="1400" noProof="0" dirty="0" err="1"/>
+            <a:t>hab.día</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-EC" sz="1400" noProof="0" dirty="0"/>
+            <a:t> *</a:t>
+          </a:r>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{64F4A272-3B11-224F-9BCE-E8B1FFFBF329}" type="parTrans" cxnId="{48B453F9-8F9E-E649-A4FD-1CC797FE0769}">
+      <dgm:prSet/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{906ABFD1-D290-054E-9489-291D41EBD670}" type="sibTrans" cxnId="{48B453F9-8F9E-E649-A4FD-1CC797FE0769}">
+      <dgm:prSet/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{17E4CF11-FB0E-C949-A6F5-6B428BD6B194}">
+      <dgm:prSet phldrT="[Text]" custT="1"/>
+      <dgm:spPr>
+        <a:solidFill>
+          <a:srgbClr val="38C566">
+            <a:alpha val="90000"/>
+          </a:srgbClr>
+        </a:solidFill>
+      </dgm:spPr>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="es-EC" sz="2000" noProof="0" dirty="0"/>
+            <a:t>GAD Micro</a:t>
+          </a:r>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{EA26D911-164D-4D4C-A288-42E6489FD24B}" type="parTrans" cxnId="{A1D8BBE3-6122-0843-A318-8D0A148EA123}">
+      <dgm:prSet/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{90F9A3FD-63B4-B14E-A7AA-4B869E5C2E97}" type="sibTrans" cxnId="{A1D8BBE3-6122-0843-A318-8D0A148EA123}">
+      <dgm:prSet/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{C7A5B271-B84C-CC4D-99CA-21772D34F961}">
+      <dgm:prSet custT="1"/>
+      <dgm:spPr>
+        <a:solidFill>
+          <a:srgbClr val="37C9D3"/>
+        </a:solidFill>
+      </dgm:spPr>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-EC" sz="1400" noProof="0" dirty="0"/>
+            <a:t>Cobertura: 80,99% **</a:t>
+          </a:r>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{E96DA78E-4AEB-E04F-B368-D297BB09B47D}" type="parTrans" cxnId="{DC32ABCE-4241-CD42-91CD-9E50EC10BDA4}">
+      <dgm:prSet/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{F5D627D0-C4B1-9745-BCFE-30571189C1F1}" type="sibTrans" cxnId="{DC32ABCE-4241-CD42-91CD-9E50EC10BDA4}">
+      <dgm:prSet/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{B0FEE185-A41D-C744-948A-D9E3BC18D0E2}">
+      <dgm:prSet phldrT="[Text]" custT="1"/>
+      <dgm:spPr>
+        <a:solidFill>
+          <a:srgbClr val="15D180"/>
+        </a:solidFill>
+      </dgm:spPr>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-EC" sz="1400" noProof="0" dirty="0"/>
+            <a:t>Cobertura: 72,87% **</a:t>
+          </a:r>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{CAB522BF-C107-054B-AEDF-DD8065489477}" type="parTrans" cxnId="{C17A41A3-EA59-7141-9328-57DE78D008F2}">
+      <dgm:prSet/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{CE82435C-F1D4-854D-8909-B60332A7F066}" type="sibTrans" cxnId="{C17A41A3-EA59-7141-9328-57DE78D008F2}">
+      <dgm:prSet/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{8786B031-BBEC-004E-B401-16E2DB877E64}">
+      <dgm:prSet phldrT="[Text]" custT="1"/>
+      <dgm:spPr>
+        <a:solidFill>
+          <a:srgbClr val="38C566"/>
+        </a:solidFill>
+      </dgm:spPr>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-EC" sz="1400" noProof="0" dirty="0"/>
+            <a:t>Cobertura: 57.60% **</a:t>
+          </a:r>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{DA254942-8769-2547-977E-B4E876539A46}" type="parTrans" cxnId="{EEC7DCF6-403F-1C46-9270-A49C351F5092}">
+      <dgm:prSet/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{FB6FEF68-AC9B-B947-818F-945BC8CB97A9}" type="sibTrans" cxnId="{EEC7DCF6-403F-1C46-9270-A49C351F5092}">
+      <dgm:prSet/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{AF756F04-A3F3-4EEF-A8F3-ADDDE9C5854F}">
+      <dgm:prSet phldrT="[Text]" custT="1"/>
+      <dgm:spPr>
+        <a:solidFill>
+          <a:srgbClr val="2B8DD9">
+            <a:alpha val="90000"/>
+          </a:srgbClr>
+        </a:solidFill>
+      </dgm:spPr>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="es-EC" sz="1800" noProof="0" dirty="0"/>
+            <a:t>GAD Especial</a:t>
+          </a:r>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{85A410CD-FFA7-4721-A0E8-1CC80BA4261B}" type="parTrans" cxnId="{DBECBF7F-19DB-4913-81BE-42478AF7FF2C}">
+      <dgm:prSet/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="es-EC"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{B5111266-FF0D-431F-BBF9-66C7F1A6FF8E}" type="sibTrans" cxnId="{DBECBF7F-19DB-4913-81BE-42478AF7FF2C}">
+      <dgm:prSet/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="es-EC"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{65D23040-8FE7-4CE8-B20B-0BE3B87B6BAF}">
+      <dgm:prSet phldrT="[Text]" custT="1"/>
+      <dgm:spPr>
+        <a:solidFill>
+          <a:srgbClr val="2B8DD9">
+            <a:alpha val="90000"/>
+          </a:srgbClr>
+        </a:solidFill>
+      </dgm:spPr>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-EC" sz="1400" noProof="0" dirty="0"/>
+            <a:t>PPC: 0,98 kg/hab.día *</a:t>
+          </a:r>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{FA6BC49E-B909-4F4E-90B5-3023E434653A}" type="parTrans" cxnId="{55336144-2B5A-48B0-9A6D-F3332C81F869}">
+      <dgm:prSet/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="es-EC"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{6A5323B1-617F-4DF1-A80A-51FD5043D7F4}" type="sibTrans" cxnId="{55336144-2B5A-48B0-9A6D-F3332C81F869}">
+      <dgm:prSet/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="es-EC"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{288BCB4C-C7A2-42E4-B321-52FBF1683073}">
+      <dgm:prSet phldrT="[Text]" custT="1"/>
+      <dgm:spPr>
+        <a:solidFill>
+          <a:srgbClr val="2B8DD9"/>
+        </a:solidFill>
+      </dgm:spPr>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-EC" sz="1400" noProof="0" dirty="0"/>
+            <a:t>Cobertura: 94.29% **</a:t>
+          </a:r>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{45FE9F1F-ABBF-4D9A-AB42-A83F8F05B67C}" type="parTrans" cxnId="{14A5004C-F46E-41A7-A986-C7BB24F87310}">
+      <dgm:prSet/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="es-EC"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{D758FBBE-BE06-4955-ACCC-DBAB44ACA41E}" type="sibTrans" cxnId="{14A5004C-F46E-41A7-A986-C7BB24F87310}">
+      <dgm:prSet/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="es-EC"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{59B3B96E-3741-456F-A9EF-563DDEA6A387}">
+      <dgm:prSet phldrT="[Text]" custT="1"/>
+      <dgm:spPr>
+        <a:solidFill>
+          <a:srgbClr val="38C566">
+            <a:alpha val="90000"/>
+          </a:srgbClr>
+        </a:solidFill>
+      </dgm:spPr>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-EC" sz="1400" noProof="0" dirty="0"/>
+            <a:t>PPC: 0.56 kg/</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-EC" sz="1400" noProof="0" dirty="0" err="1"/>
+            <a:t>hab.día</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-EC" sz="1400" noProof="0" dirty="0"/>
+            <a:t> *</a:t>
+          </a:r>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{9E9CF621-4D2A-43CF-9403-8694FDBC61F3}" type="parTrans" cxnId="{0BC6D809-3186-4D17-B48A-8750B53F37E9}">
+      <dgm:prSet/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="es-EC"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{6009877E-1747-48D3-A911-016F9DC5268F}" type="sibTrans" cxnId="{0BC6D809-3186-4D17-B48A-8750B53F37E9}">
+      <dgm:prSet/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="es-EC"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{C7DEF7FE-8B4C-594C-92CF-560C3DC2E911}" type="pres">
+      <dgm:prSet presAssocID="{3D58A12A-B9B8-264E-BD9E-E85FA3CBA9EA}" presName="Name0" presStyleCnt="0">
+        <dgm:presLayoutVars>
+          <dgm:dir/>
+          <dgm:animLvl val="lvl"/>
+          <dgm:resizeHandles val="exact"/>
+        </dgm:presLayoutVars>
+      </dgm:prSet>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="es-EC"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{9C7BD3E5-68BC-4189-AAB8-658CE0345833}" type="pres">
+      <dgm:prSet presAssocID="{AF756F04-A3F3-4EEF-A8F3-ADDDE9C5854F}" presName="linNode" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{813A54B4-3135-47CE-A174-3B2D3D4B534E}" type="pres">
+      <dgm:prSet presAssocID="{AF756F04-A3F3-4EEF-A8F3-ADDDE9C5854F}" presName="parentText" presStyleLbl="node1" presStyleIdx="0" presStyleCnt="5" custScaleY="158903">
+        <dgm:presLayoutVars>
+          <dgm:chMax val="1"/>
+          <dgm:bulletEnabled val="1"/>
+        </dgm:presLayoutVars>
+      </dgm:prSet>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="es-EC"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{B9957E0A-07BC-416C-A1DB-F10357D43D61}" type="pres">
+      <dgm:prSet presAssocID="{AF756F04-A3F3-4EEF-A8F3-ADDDE9C5854F}" presName="descendantText" presStyleLbl="alignAccFollowNode1" presStyleIdx="0" presStyleCnt="5" custScaleY="219348" custLinFactNeighborX="639" custLinFactNeighborY="-43904">
+        <dgm:presLayoutVars>
+          <dgm:bulletEnabled val="1"/>
+        </dgm:presLayoutVars>
+      </dgm:prSet>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="es-EC"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{7540C69C-2169-44FE-ADCE-8E23502DCBD3}" type="pres">
+      <dgm:prSet presAssocID="{B5111266-FF0D-431F-BBF9-66C7F1A6FF8E}" presName="sp" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{595E6BE8-07B2-A24A-AB0B-D20BB10BCAFA}" type="pres">
+      <dgm:prSet presAssocID="{E198C860-F583-3A45-B783-2F1B64498303}" presName="linNode" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{91549FCC-E9A0-B141-9774-A923F7381D2C}" type="pres">
+      <dgm:prSet presAssocID="{E198C860-F583-3A45-B783-2F1B64498303}" presName="parentText" presStyleLbl="node1" presStyleIdx="1" presStyleCnt="5" custScaleY="173758">
+        <dgm:presLayoutVars>
+          <dgm:chMax val="1"/>
+          <dgm:bulletEnabled val="1"/>
+        </dgm:presLayoutVars>
+      </dgm:prSet>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="es-EC"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{5D650F7A-BFE6-DB4A-9105-E6E4F5F41C22}" type="pres">
+      <dgm:prSet presAssocID="{E198C860-F583-3A45-B783-2F1B64498303}" presName="descendantText" presStyleLbl="alignAccFollowNode1" presStyleIdx="1" presStyleCnt="5" custScaleY="228535">
+        <dgm:presLayoutVars>
+          <dgm:bulletEnabled val="1"/>
+        </dgm:presLayoutVars>
+      </dgm:prSet>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="es-EC"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{97830D75-5FBD-5748-854F-D54FFE7A529F}" type="pres">
+      <dgm:prSet presAssocID="{6EBA461A-EF40-7C42-808C-13AB114788E8}" presName="sp" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{B7A87240-B48D-5F48-B158-74DA4F6C8380}" type="pres">
+      <dgm:prSet presAssocID="{3B22AF23-C402-284E-94ED-F6615174E79D}" presName="linNode" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{CDA767FF-EAED-DB47-940B-5DAF300473EF}" type="pres">
+      <dgm:prSet presAssocID="{3B22AF23-C402-284E-94ED-F6615174E79D}" presName="parentText" presStyleLbl="node1" presStyleIdx="2" presStyleCnt="5" custScaleY="158175">
+        <dgm:presLayoutVars>
+          <dgm:chMax val="1"/>
+          <dgm:bulletEnabled val="1"/>
+        </dgm:presLayoutVars>
+      </dgm:prSet>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="es-EC"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{559308A9-B2DA-C74B-997E-3C2A17F7D843}" type="pres">
+      <dgm:prSet presAssocID="{3B22AF23-C402-284E-94ED-F6615174E79D}" presName="descendantText" presStyleLbl="alignAccFollowNode1" presStyleIdx="2" presStyleCnt="5" custScaleY="197526">
+        <dgm:presLayoutVars>
+          <dgm:bulletEnabled val="1"/>
+        </dgm:presLayoutVars>
+      </dgm:prSet>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="es-EC"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{9ECFDBB3-6FDC-9746-82EB-4D9EA2B13284}" type="pres">
+      <dgm:prSet presAssocID="{D4B4AB0A-4AB5-034E-AEA2-8BFBB76563F6}" presName="sp" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{D6AF9926-118A-4F4A-931C-CE11B48532DB}" type="pres">
+      <dgm:prSet presAssocID="{ECB1009C-45F1-AD49-8507-8844A4E0AC68}" presName="linNode" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{7390C052-D57F-2345-A59A-DC77BC341A28}" type="pres">
+      <dgm:prSet presAssocID="{ECB1009C-45F1-AD49-8507-8844A4E0AC68}" presName="parentText" presStyleLbl="node1" presStyleIdx="3" presStyleCnt="5" custScaleY="150983">
+        <dgm:presLayoutVars>
+          <dgm:chMax val="1"/>
+          <dgm:bulletEnabled val="1"/>
+        </dgm:presLayoutVars>
+      </dgm:prSet>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="es-EC"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{D65C2623-45BD-DC45-B1B1-AD2A2C5740C3}" type="pres">
+      <dgm:prSet presAssocID="{ECB1009C-45F1-AD49-8507-8844A4E0AC68}" presName="descendantText" presStyleLbl="alignAccFollowNode1" presStyleIdx="3" presStyleCnt="5" custScaleY="203148">
+        <dgm:presLayoutVars>
+          <dgm:bulletEnabled val="1"/>
+        </dgm:presLayoutVars>
+      </dgm:prSet>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="es-EC"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{C6E21C76-4BC8-9E43-B2AB-ECBC70D75A09}" type="pres">
+      <dgm:prSet presAssocID="{CE595159-41CD-D443-8F5F-79EF4DC30577}" presName="sp" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{FD76C001-9DCC-554F-8A36-A8E7F7E927B8}" type="pres">
+      <dgm:prSet presAssocID="{17E4CF11-FB0E-C949-A6F5-6B428BD6B194}" presName="linNode" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{45D2AFDD-45CA-754B-AA43-693B437746E5}" type="pres">
+      <dgm:prSet presAssocID="{17E4CF11-FB0E-C949-A6F5-6B428BD6B194}" presName="parentText" presStyleLbl="node1" presStyleIdx="4" presStyleCnt="5" custScaleY="151215">
+        <dgm:presLayoutVars>
+          <dgm:chMax val="1"/>
+          <dgm:bulletEnabled val="1"/>
+        </dgm:presLayoutVars>
+      </dgm:prSet>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="es-EC"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{E2722DC5-7D56-0D41-A1F0-8943119E8838}" type="pres">
+      <dgm:prSet presAssocID="{17E4CF11-FB0E-C949-A6F5-6B428BD6B194}" presName="descendantText" presStyleLbl="alignAccFollowNode1" presStyleIdx="4" presStyleCnt="5" custScaleY="218664">
+        <dgm:presLayoutVars>
+          <dgm:bulletEnabled val="1"/>
+        </dgm:presLayoutVars>
+      </dgm:prSet>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="es-EC"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+  </dgm:ptLst>
+  <dgm:cxnLst>
+    <dgm:cxn modelId="{F8434D64-C311-A743-95CC-1EED8CCDDBF9}" srcId="{E198C860-F583-3A45-B783-2F1B64498303}" destId="{541570D1-BB87-5142-A402-22840FAA1C66}" srcOrd="0" destOrd="0" parTransId="{D899A435-369B-3641-96A7-864ED0FE03AD}" sibTransId="{17AC0375-E1CE-3940-82EE-7586D4188233}"/>
+    <dgm:cxn modelId="{36671E8B-3A1B-4F95-B2D5-A1C26DAAFB03}" type="presOf" srcId="{B0FEE185-A41D-C744-948A-D9E3BC18D0E2}" destId="{D65C2623-45BD-DC45-B1B1-AD2A2C5740C3}" srcOrd="0" destOrd="1" presId="urn:microsoft.com/office/officeart/2005/8/layout/vList5"/>
+    <dgm:cxn modelId="{78015659-769D-4FE0-ABBC-906B3D2AFC07}" type="presOf" srcId="{4B9D3448-F1F1-A64B-B475-FF5B1414BA51}" destId="{559308A9-B2DA-C74B-997E-3C2A17F7D843}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/vList5"/>
+    <dgm:cxn modelId="{D4A9EAFB-8EFA-A844-9109-55519A64765F}" srcId="{3B22AF23-C402-284E-94ED-F6615174E79D}" destId="{4B9D3448-F1F1-A64B-B475-FF5B1414BA51}" srcOrd="0" destOrd="0" parTransId="{908EBDA6-70C5-B248-A16B-7D0276715C37}" sibTransId="{5C186B2D-E6AB-EF4D-B949-98ED92504A65}"/>
+    <dgm:cxn modelId="{DBECBF7F-19DB-4913-81BE-42478AF7FF2C}" srcId="{3D58A12A-B9B8-264E-BD9E-E85FA3CBA9EA}" destId="{AF756F04-A3F3-4EEF-A8F3-ADDDE9C5854F}" srcOrd="0" destOrd="0" parTransId="{85A410CD-FFA7-4721-A0E8-1CC80BA4261B}" sibTransId="{B5111266-FF0D-431F-BBF9-66C7F1A6FF8E}"/>
+    <dgm:cxn modelId="{2E0A4BCC-A4B1-7144-B28A-D0A45104CA3B}" srcId="{E198C860-F583-3A45-B783-2F1B64498303}" destId="{7A9F7AFA-C04E-BD4D-82F0-C72444B4257E}" srcOrd="1" destOrd="0" parTransId="{6543371B-5BBE-4743-BE56-5A7F7669D274}" sibTransId="{C427DA95-AF77-2349-8B32-BE493CCB5CE3}"/>
+    <dgm:cxn modelId="{55336144-2B5A-48B0-9A6D-F3332C81F869}" srcId="{AF756F04-A3F3-4EEF-A8F3-ADDDE9C5854F}" destId="{65D23040-8FE7-4CE8-B20B-0BE3B87B6BAF}" srcOrd="0" destOrd="0" parTransId="{FA6BC49E-B909-4F4E-90B5-3023E434653A}" sibTransId="{6A5323B1-617F-4DF1-A80A-51FD5043D7F4}"/>
+    <dgm:cxn modelId="{EEC7DCF6-403F-1C46-9270-A49C351F5092}" srcId="{17E4CF11-FB0E-C949-A6F5-6B428BD6B194}" destId="{8786B031-BBEC-004E-B401-16E2DB877E64}" srcOrd="1" destOrd="0" parTransId="{DA254942-8769-2547-977E-B4E876539A46}" sibTransId="{FB6FEF68-AC9B-B947-818F-945BC8CB97A9}"/>
+    <dgm:cxn modelId="{DC32ABCE-4241-CD42-91CD-9E50EC10BDA4}" srcId="{3B22AF23-C402-284E-94ED-F6615174E79D}" destId="{C7A5B271-B84C-CC4D-99CA-21772D34F961}" srcOrd="1" destOrd="0" parTransId="{E96DA78E-4AEB-E04F-B368-D297BB09B47D}" sibTransId="{F5D627D0-C4B1-9745-BCFE-30571189C1F1}"/>
+    <dgm:cxn modelId="{7520AB30-FB55-487F-BC27-02446F072CCC}" type="presOf" srcId="{C7A5B271-B84C-CC4D-99CA-21772D34F961}" destId="{559308A9-B2DA-C74B-997E-3C2A17F7D843}" srcOrd="0" destOrd="1" presId="urn:microsoft.com/office/officeart/2005/8/layout/vList5"/>
+    <dgm:cxn modelId="{2C88A80D-CCF8-4F6A-9CBB-DD12A9D17758}" type="presOf" srcId="{8786B031-BBEC-004E-B401-16E2DB877E64}" destId="{E2722DC5-7D56-0D41-A1F0-8943119E8838}" srcOrd="0" destOrd="1" presId="urn:microsoft.com/office/officeart/2005/8/layout/vList5"/>
+    <dgm:cxn modelId="{418D43B8-196E-4C94-9943-94C8E8D3D7FC}" type="presOf" srcId="{FC7B3C0A-79EE-C043-98FB-AA5109650539}" destId="{D65C2623-45BD-DC45-B1B1-AD2A2C5740C3}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/vList5"/>
+    <dgm:cxn modelId="{3DDB7960-FB2B-4D5F-A6AA-D19DD1E63814}" type="presOf" srcId="{3B22AF23-C402-284E-94ED-F6615174E79D}" destId="{CDA767FF-EAED-DB47-940B-5DAF300473EF}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/vList5"/>
+    <dgm:cxn modelId="{3FA8B827-CE26-AB4E-AFEA-A2D349DC1784}" srcId="{3D58A12A-B9B8-264E-BD9E-E85FA3CBA9EA}" destId="{3B22AF23-C402-284E-94ED-F6615174E79D}" srcOrd="2" destOrd="0" parTransId="{4444906B-EB1F-D14E-AFB8-F39CE987C67F}" sibTransId="{D4B4AB0A-4AB5-034E-AEA2-8BFBB76563F6}"/>
+    <dgm:cxn modelId="{3E1465CE-D3A8-4EAA-B3F8-0BA3C1CE07DC}" type="presOf" srcId="{65D23040-8FE7-4CE8-B20B-0BE3B87B6BAF}" destId="{B9957E0A-07BC-416C-A1DB-F10357D43D61}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/vList5"/>
+    <dgm:cxn modelId="{A1D8BBE3-6122-0843-A318-8D0A148EA123}" srcId="{3D58A12A-B9B8-264E-BD9E-E85FA3CBA9EA}" destId="{17E4CF11-FB0E-C949-A6F5-6B428BD6B194}" srcOrd="4" destOrd="0" parTransId="{EA26D911-164D-4D4C-A288-42E6489FD24B}" sibTransId="{90F9A3FD-63B4-B14E-A7AA-4B869E5C2E97}"/>
+    <dgm:cxn modelId="{14A5004C-F46E-41A7-A986-C7BB24F87310}" srcId="{AF756F04-A3F3-4EEF-A8F3-ADDDE9C5854F}" destId="{288BCB4C-C7A2-42E4-B321-52FBF1683073}" srcOrd="1" destOrd="0" parTransId="{45FE9F1F-ABBF-4D9A-AB42-A83F8F05B67C}" sibTransId="{D758FBBE-BE06-4955-ACCC-DBAB44ACA41E}"/>
+    <dgm:cxn modelId="{4B82F0EE-365F-42F1-98A8-C52BA648623A}" type="presOf" srcId="{ECB1009C-45F1-AD49-8507-8844A4E0AC68}" destId="{7390C052-D57F-2345-A59A-DC77BC341A28}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/vList5"/>
+    <dgm:cxn modelId="{25A2464D-DC47-47DC-99A2-18F00938184D}" type="presOf" srcId="{E198C860-F583-3A45-B783-2F1B64498303}" destId="{91549FCC-E9A0-B141-9774-A923F7381D2C}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/vList5"/>
+    <dgm:cxn modelId="{C262E6E3-9D2A-450A-9322-696C23356DA0}" type="presOf" srcId="{7A9F7AFA-C04E-BD4D-82F0-C72444B4257E}" destId="{5D650F7A-BFE6-DB4A-9105-E6E4F5F41C22}" srcOrd="0" destOrd="1" presId="urn:microsoft.com/office/officeart/2005/8/layout/vList5"/>
+    <dgm:cxn modelId="{E038AD93-4DA8-49E4-9A66-1AB420248EC2}" type="presOf" srcId="{AF756F04-A3F3-4EEF-A8F3-ADDDE9C5854F}" destId="{813A54B4-3135-47CE-A174-3B2D3D4B534E}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/vList5"/>
+    <dgm:cxn modelId="{1AABC88E-F99A-469A-8C15-621EAF108851}" type="presOf" srcId="{288BCB4C-C7A2-42E4-B321-52FBF1683073}" destId="{B9957E0A-07BC-416C-A1DB-F10357D43D61}" srcOrd="0" destOrd="1" presId="urn:microsoft.com/office/officeart/2005/8/layout/vList5"/>
+    <dgm:cxn modelId="{B92E82A1-2AC9-1E46-9B77-DA221A30937C}" srcId="{3D58A12A-B9B8-264E-BD9E-E85FA3CBA9EA}" destId="{E198C860-F583-3A45-B783-2F1B64498303}" srcOrd="1" destOrd="0" parTransId="{AEB4A8E4-1F1E-D84E-B712-6CFC524438EE}" sibTransId="{6EBA461A-EF40-7C42-808C-13AB114788E8}"/>
+    <dgm:cxn modelId="{1EAF92B2-8F95-4F5A-8145-12676C2860E4}" type="presOf" srcId="{17E4CF11-FB0E-C949-A6F5-6B428BD6B194}" destId="{45D2AFDD-45CA-754B-AA43-693B437746E5}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/vList5"/>
+    <dgm:cxn modelId="{A27A416A-3F9E-4E14-AA72-A35E5922D613}" type="presOf" srcId="{3D58A12A-B9B8-264E-BD9E-E85FA3CBA9EA}" destId="{C7DEF7FE-8B4C-594C-92CF-560C3DC2E911}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/vList5"/>
+    <dgm:cxn modelId="{48B453F9-8F9E-E649-A4FD-1CC797FE0769}" srcId="{ECB1009C-45F1-AD49-8507-8844A4E0AC68}" destId="{FC7B3C0A-79EE-C043-98FB-AA5109650539}" srcOrd="0" destOrd="0" parTransId="{64F4A272-3B11-224F-9BCE-E8B1FFFBF329}" sibTransId="{906ABFD1-D290-054E-9489-291D41EBD670}"/>
+    <dgm:cxn modelId="{0BC6D809-3186-4D17-B48A-8750B53F37E9}" srcId="{17E4CF11-FB0E-C949-A6F5-6B428BD6B194}" destId="{59B3B96E-3741-456F-A9EF-563DDEA6A387}" srcOrd="0" destOrd="0" parTransId="{9E9CF621-4D2A-43CF-9403-8694FDBC61F3}" sibTransId="{6009877E-1747-48D3-A911-016F9DC5268F}"/>
+    <dgm:cxn modelId="{DF28298D-C9F3-2147-85E8-D39D967E3067}" srcId="{3D58A12A-B9B8-264E-BD9E-E85FA3CBA9EA}" destId="{ECB1009C-45F1-AD49-8507-8844A4E0AC68}" srcOrd="3" destOrd="0" parTransId="{E14009BB-621C-2A41-A673-C557A1CA377B}" sibTransId="{CE595159-41CD-D443-8F5F-79EF4DC30577}"/>
+    <dgm:cxn modelId="{29BC52BC-DC48-41DA-A13F-DC431FDDFD8A}" type="presOf" srcId="{59B3B96E-3741-456F-A9EF-563DDEA6A387}" destId="{E2722DC5-7D56-0D41-A1F0-8943119E8838}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/vList5"/>
+    <dgm:cxn modelId="{7006DEEA-C6F4-40B4-82A0-A5D6042C51EC}" type="presOf" srcId="{541570D1-BB87-5142-A402-22840FAA1C66}" destId="{5D650F7A-BFE6-DB4A-9105-E6E4F5F41C22}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/vList5"/>
+    <dgm:cxn modelId="{C17A41A3-EA59-7141-9328-57DE78D008F2}" srcId="{ECB1009C-45F1-AD49-8507-8844A4E0AC68}" destId="{B0FEE185-A41D-C744-948A-D9E3BC18D0E2}" srcOrd="1" destOrd="0" parTransId="{CAB522BF-C107-054B-AEDF-DD8065489477}" sibTransId="{CE82435C-F1D4-854D-8909-B60332A7F066}"/>
+    <dgm:cxn modelId="{54B91CD5-C660-40F5-8B27-34048EC4AB30}" type="presParOf" srcId="{C7DEF7FE-8B4C-594C-92CF-560C3DC2E911}" destId="{9C7BD3E5-68BC-4189-AAB8-658CE0345833}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/vList5"/>
+    <dgm:cxn modelId="{C0B69673-3F83-42DE-810D-52258D553854}" type="presParOf" srcId="{9C7BD3E5-68BC-4189-AAB8-658CE0345833}" destId="{813A54B4-3135-47CE-A174-3B2D3D4B534E}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/vList5"/>
+    <dgm:cxn modelId="{A1208B42-028C-4C53-B8BD-920078142001}" type="presParOf" srcId="{9C7BD3E5-68BC-4189-AAB8-658CE0345833}" destId="{B9957E0A-07BC-416C-A1DB-F10357D43D61}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/vList5"/>
+    <dgm:cxn modelId="{9B5FE98B-A20F-40C9-ACE6-62191C195970}" type="presParOf" srcId="{C7DEF7FE-8B4C-594C-92CF-560C3DC2E911}" destId="{7540C69C-2169-44FE-ADCE-8E23502DCBD3}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/vList5"/>
+    <dgm:cxn modelId="{A9AAE817-CDA9-4408-A1D1-9BC55E13B053}" type="presParOf" srcId="{C7DEF7FE-8B4C-594C-92CF-560C3DC2E911}" destId="{595E6BE8-07B2-A24A-AB0B-D20BB10BCAFA}" srcOrd="2" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/vList5"/>
+    <dgm:cxn modelId="{C6885793-B2B2-45FA-8A43-DE318F289F1F}" type="presParOf" srcId="{595E6BE8-07B2-A24A-AB0B-D20BB10BCAFA}" destId="{91549FCC-E9A0-B141-9774-A923F7381D2C}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/vList5"/>
+    <dgm:cxn modelId="{A546AC0D-BCB4-48DE-B724-C84C5010AB88}" type="presParOf" srcId="{595E6BE8-07B2-A24A-AB0B-D20BB10BCAFA}" destId="{5D650F7A-BFE6-DB4A-9105-E6E4F5F41C22}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/vList5"/>
+    <dgm:cxn modelId="{95041EF2-7D83-4609-8C2A-3C826CACC489}" type="presParOf" srcId="{C7DEF7FE-8B4C-594C-92CF-560C3DC2E911}" destId="{97830D75-5FBD-5748-854F-D54FFE7A529F}" srcOrd="3" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/vList5"/>
+    <dgm:cxn modelId="{9227C39B-36F3-40A3-BA04-D2CB28E2CB2F}" type="presParOf" srcId="{C7DEF7FE-8B4C-594C-92CF-560C3DC2E911}" destId="{B7A87240-B48D-5F48-B158-74DA4F6C8380}" srcOrd="4" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/vList5"/>
+    <dgm:cxn modelId="{7E83E1F7-2CF4-40F0-9D69-7507CDEFB55E}" type="presParOf" srcId="{B7A87240-B48D-5F48-B158-74DA4F6C8380}" destId="{CDA767FF-EAED-DB47-940B-5DAF300473EF}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/vList5"/>
+    <dgm:cxn modelId="{A91FEF8F-C06E-4684-85BA-F43DF0B0F36C}" type="presParOf" srcId="{B7A87240-B48D-5F48-B158-74DA4F6C8380}" destId="{559308A9-B2DA-C74B-997E-3C2A17F7D843}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/vList5"/>
+    <dgm:cxn modelId="{A7B329A3-CD8F-4B54-BEBB-1A216C17D20C}" type="presParOf" srcId="{C7DEF7FE-8B4C-594C-92CF-560C3DC2E911}" destId="{9ECFDBB3-6FDC-9746-82EB-4D9EA2B13284}" srcOrd="5" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/vList5"/>
+    <dgm:cxn modelId="{2C663DEB-9493-4C4E-AC55-D1422290BF2D}" type="presParOf" srcId="{C7DEF7FE-8B4C-594C-92CF-560C3DC2E911}" destId="{D6AF9926-118A-4F4A-931C-CE11B48532DB}" srcOrd="6" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/vList5"/>
+    <dgm:cxn modelId="{5619E0AF-B28D-465E-A271-CF69BB25F825}" type="presParOf" srcId="{D6AF9926-118A-4F4A-931C-CE11B48532DB}" destId="{7390C052-D57F-2345-A59A-DC77BC341A28}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/vList5"/>
+    <dgm:cxn modelId="{66F2A892-82D3-4337-8116-2A3810F4DC52}" type="presParOf" srcId="{D6AF9926-118A-4F4A-931C-CE11B48532DB}" destId="{D65C2623-45BD-DC45-B1B1-AD2A2C5740C3}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/vList5"/>
+    <dgm:cxn modelId="{15BED68E-ED41-4A18-A557-9336EED93890}" type="presParOf" srcId="{C7DEF7FE-8B4C-594C-92CF-560C3DC2E911}" destId="{C6E21C76-4BC8-9E43-B2AB-ECBC70D75A09}" srcOrd="7" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/vList5"/>
+    <dgm:cxn modelId="{F5EFB9AC-EAB9-46DE-B4FB-549BC5EB9598}" type="presParOf" srcId="{C7DEF7FE-8B4C-594C-92CF-560C3DC2E911}" destId="{FD76C001-9DCC-554F-8A36-A8E7F7E927B8}" srcOrd="8" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/vList5"/>
+    <dgm:cxn modelId="{41D6D5AB-84D8-4BB0-8B79-FC549B313A15}" type="presParOf" srcId="{FD76C001-9DCC-554F-8A36-A8E7F7E927B8}" destId="{45D2AFDD-45CA-754B-AA43-693B437746E5}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/vList5"/>
+    <dgm:cxn modelId="{B7EB0E0D-3ACF-43DC-BD61-6852D592B188}" type="presParOf" srcId="{FD76C001-9DCC-554F-8A36-A8E7F7E927B8}" destId="{E2722DC5-7D56-0D41-A1F0-8943119E8838}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/vList5"/>
+  </dgm:cxnLst>
+  <dgm:bg/>
+  <dgm:whole/>
+  <dgm:extLst>
+    <a:ext uri="http://schemas.microsoft.com/office/drawing/2008/diagram">
+      <dsp:dataModelExt xmlns:dsp="http://schemas.microsoft.com/office/drawing/2008/diagram" relId="rId5" minVer="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+    </a:ext>
+  </dgm:extLst>
+</dgm:dataModel>
+</file>
+
+<file path=xl/diagrams/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<dsp:drawing xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:dsp="http://schemas.microsoft.com/office/drawing/2008/diagram" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <dsp:spTree>
+    <dsp:nvGrpSpPr>
+      <dsp:cNvPr id="0" name=""/>
+      <dsp:cNvGrpSpPr/>
+    </dsp:nvGrpSpPr>
+    <dsp:grpSpPr/>
+  </dsp:spTree>
+</dsp:drawing>
+</file>
+
+<file path=xl/diagrams/layout1.xml><?xml version="1.0" encoding="utf-8"?>
+<dgm:layoutDef xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uniqueId="urn:microsoft.com/office/officeart/2005/8/layout/vList5">
+  <dgm:title val=""/>
+  <dgm:desc val=""/>
+  <dgm:catLst>
+    <dgm:cat type="list" pri="15000"/>
+    <dgm:cat type="convert" pri="2000"/>
+  </dgm:catLst>
+  <dgm:sampData>
+    <dgm:dataModel>
+      <dgm:ptLst>
+        <dgm:pt modelId="0" type="doc"/>
+        <dgm:pt modelId="1">
+          <dgm:prSet phldr="1"/>
+        </dgm:pt>
+        <dgm:pt modelId="11">
+          <dgm:prSet phldr="1"/>
+        </dgm:pt>
+        <dgm:pt modelId="12">
+          <dgm:prSet phldr="1"/>
+        </dgm:pt>
+        <dgm:pt modelId="2">
+          <dgm:prSet phldr="1"/>
+        </dgm:pt>
+        <dgm:pt modelId="21">
+          <dgm:prSet phldr="1"/>
+        </dgm:pt>
+        <dgm:pt modelId="22">
+          <dgm:prSet phldr="1"/>
+        </dgm:pt>
+        <dgm:pt modelId="3">
+          <dgm:prSet phldr="1"/>
+        </dgm:pt>
+        <dgm:pt modelId="31">
+          <dgm:prSet phldr="1"/>
+        </dgm:pt>
+        <dgm:pt modelId="32">
+          <dgm:prSet phldr="1"/>
+        </dgm:pt>
+      </dgm:ptLst>
+      <dgm:cxnLst>
+        <dgm:cxn modelId="4" srcId="0" destId="1" srcOrd="0" destOrd="0"/>
+        <dgm:cxn modelId="5" srcId="0" destId="2" srcOrd="1" destOrd="0"/>
+        <dgm:cxn modelId="6" srcId="0" destId="3" srcOrd="2" destOrd="0"/>
+        <dgm:cxn modelId="13" srcId="1" destId="11" srcOrd="0" destOrd="0"/>
+        <dgm:cxn modelId="14" srcId="1" destId="12" srcOrd="1" destOrd="0"/>
+        <dgm:cxn modelId="23" srcId="2" destId="21" srcOrd="0" destOrd="0"/>
+        <dgm:cxn modelId="24" srcId="2" destId="22" srcOrd="1" destOrd="0"/>
+        <dgm:cxn modelId="33" srcId="3" destId="31" srcOrd="0" destOrd="0"/>
+        <dgm:cxn modelId="34" srcId="3" destId="32" srcOrd="1" destOrd="0"/>
+      </dgm:cxnLst>
+      <dgm:bg/>
+      <dgm:whole/>
+    </dgm:dataModel>
+  </dgm:sampData>
+  <dgm:styleData>
+    <dgm:dataModel>
+      <dgm:ptLst>
+        <dgm:pt modelId="0" type="doc"/>
+        <dgm:pt modelId="1"/>
+        <dgm:pt modelId="11"/>
+        <dgm:pt modelId="2"/>
+        <dgm:pt modelId="21"/>
+      </dgm:ptLst>
+      <dgm:cxnLst>
+        <dgm:cxn modelId="4" srcId="0" destId="1" srcOrd="0" destOrd="0"/>
+        <dgm:cxn modelId="5" srcId="0" destId="2" srcOrd="1" destOrd="0"/>
+        <dgm:cxn modelId="13" srcId="1" destId="11" srcOrd="0" destOrd="0"/>
+        <dgm:cxn modelId="23" srcId="2" destId="21" srcOrd="0" destOrd="0"/>
+      </dgm:cxnLst>
+      <dgm:bg/>
+      <dgm:whole/>
+    </dgm:dataModel>
+  </dgm:styleData>
+  <dgm:clrData>
+    <dgm:dataModel>
+      <dgm:ptLst>
+        <dgm:pt modelId="0" type="doc"/>
+        <dgm:pt modelId="1"/>
+        <dgm:pt modelId="11"/>
+        <dgm:pt modelId="2"/>
+        <dgm:pt modelId="21"/>
+        <dgm:pt modelId="3"/>
+        <dgm:pt modelId="31"/>
+        <dgm:pt modelId="4"/>
+        <dgm:pt modelId="41"/>
+      </dgm:ptLst>
+      <dgm:cxnLst>
+        <dgm:cxn modelId="5" srcId="0" destId="1" srcOrd="0" destOrd="0"/>
+        <dgm:cxn modelId="6" srcId="0" destId="2" srcOrd="1" destOrd="0"/>
+        <dgm:cxn modelId="7" srcId="0" destId="3" srcOrd="2" destOrd="0"/>
+        <dgm:cxn modelId="8" srcId="0" destId="4" srcOrd="3" destOrd="0"/>
+        <dgm:cxn modelId="13" srcId="1" destId="11" srcOrd="0" destOrd="0"/>
+        <dgm:cxn modelId="23" srcId="2" destId="21" srcOrd="0" destOrd="0"/>
+        <dgm:cxn modelId="33" srcId="3" destId="31" srcOrd="0" destOrd="0"/>
+        <dgm:cxn modelId="43" srcId="4" destId="41" srcOrd="0" destOrd="0"/>
+      </dgm:cxnLst>
+      <dgm:bg/>
+      <dgm:whole/>
+    </dgm:dataModel>
+  </dgm:clrData>
+  <dgm:layoutNode name="Name0">
+    <dgm:varLst>
+      <dgm:dir/>
+      <dgm:animLvl val="lvl"/>
+      <dgm:resizeHandles val="exact"/>
+    </dgm:varLst>
+    <dgm:choose name="Name1">
+      <dgm:if name="Name2" func="var" arg="dir" op="equ" val="norm">
+        <dgm:alg type="lin">
+          <dgm:param type="linDir" val="fromT"/>
+          <dgm:param type="nodeHorzAlign" val="l"/>
+        </dgm:alg>
+      </dgm:if>
+      <dgm:else name="Name3">
+        <dgm:alg type="lin">
+          <dgm:param type="linDir" val="fromT"/>
+          <dgm:param type="nodeHorzAlign" val="r"/>
+        </dgm:alg>
+      </dgm:else>
+    </dgm:choose>
+    <dgm:shape xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:blip="">
+      <dgm:adjLst/>
+    </dgm:shape>
+    <dgm:presOf/>
+    <dgm:constrLst>
+      <dgm:constr type="h" for="ch" forName="linNode" refType="h"/>
+      <dgm:constr type="w" for="ch" forName="linNode" refType="w"/>
+      <dgm:constr type="h" for="ch" forName="sp" refType="h" fact="0.05"/>
+      <dgm:constr type="primFontSz" for="des" forName="parentText" op="equ" val="65"/>
+      <dgm:constr type="secFontSz" for="des" forName="descendantText" op="equ"/>
+    </dgm:constrLst>
+    <dgm:ruleLst/>
+    <dgm:forEach name="Name4" axis="ch" ptType="node">
+      <dgm:layoutNode name="linNode">
+        <dgm:choose name="Name5">
+          <dgm:if name="Name6" func="var" arg="dir" op="equ" val="norm">
+            <dgm:alg type="lin">
+              <dgm:param type="linDir" val="fromL"/>
+            </dgm:alg>
+          </dgm:if>
+          <dgm:else name="Name7">
+            <dgm:alg type="lin">
+              <dgm:param type="linDir" val="fromR"/>
+            </dgm:alg>
+          </dgm:else>
+        </dgm:choose>
+        <dgm:shape xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:blip="">
+          <dgm:adjLst/>
+        </dgm:shape>
+        <dgm:presOf/>
+        <dgm:constrLst>
+          <dgm:constr type="w" for="ch" forName="parentText" refType="w" fact="0.36"/>
+          <dgm:constr type="w" for="ch" forName="descendantText" refType="w" fact="0.64"/>
+          <dgm:constr type="h" for="ch" forName="parentText" refType="h"/>
+          <dgm:constr type="h" for="ch" forName="descendantText" refType="h" refFor="ch" refForName="parentText" fact="0.8"/>
+        </dgm:constrLst>
+        <dgm:ruleLst/>
+        <dgm:layoutNode name="parentText">
+          <dgm:varLst>
+            <dgm:chMax val="1"/>
+            <dgm:bulletEnabled val="1"/>
+          </dgm:varLst>
+          <dgm:alg type="tx"/>
+          <dgm:shape xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" type="roundRect" r:blip="" zOrderOff="3">
+            <dgm:adjLst/>
+          </dgm:shape>
+          <dgm:presOf axis="self" ptType="node"/>
+          <dgm:constrLst>
+            <dgm:constr type="tMarg" refType="primFontSz" fact="0.15"/>
+            <dgm:constr type="bMarg" refType="primFontSz" fact="0.15"/>
+            <dgm:constr type="lMarg" refType="primFontSz" fact="0.3"/>
+            <dgm:constr type="rMarg" refType="primFontSz" fact="0.3"/>
+          </dgm:constrLst>
+          <dgm:ruleLst>
+            <dgm:rule type="primFontSz" val="5" fact="NaN" max="NaN"/>
+          </dgm:ruleLst>
+        </dgm:layoutNode>
+        <dgm:choose name="Name8">
+          <dgm:if name="Name9" axis="ch" ptType="node" func="cnt" op="gte" val="1">
+            <dgm:layoutNode name="descendantText" styleLbl="alignAccFollowNode1">
+              <dgm:varLst>
+                <dgm:bulletEnabled val="1"/>
+              </dgm:varLst>
+              <dgm:alg type="tx">
+                <dgm:param type="stBulletLvl" val="1"/>
+                <dgm:param type="txAnchorVertCh" val="mid"/>
+              </dgm:alg>
+              <dgm:choose name="Name10">
+                <dgm:if name="Name11" func="var" arg="dir" op="equ" val="norm">
+                  <dgm:shape xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" rot="90" type="round2SameRect" r:blip="">
+                    <dgm:adjLst/>
+                  </dgm:shape>
+                </dgm:if>
+                <dgm:else name="Name12">
+                  <dgm:shape xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" rot="-90" type="round2SameRect" r:blip="">
+                    <dgm:adjLst/>
+                  </dgm:shape>
+                </dgm:else>
+              </dgm:choose>
+              <dgm:presOf axis="des" ptType="node"/>
+              <dgm:constrLst>
+                <dgm:constr type="secFontSz" val="65"/>
+                <dgm:constr type="primFontSz" refType="secFontSz"/>
+                <dgm:constr type="lMarg" refType="secFontSz" fact="0.3"/>
+                <dgm:constr type="rMarg" refType="secFontSz" fact="0.3"/>
+                <dgm:constr type="tMarg" refType="secFontSz" fact="0.15"/>
+                <dgm:constr type="bMarg" refType="secFontSz" fact="0.15"/>
+              </dgm:constrLst>
+              <dgm:ruleLst>
+                <dgm:rule type="secFontSz" val="5" fact="NaN" max="NaN"/>
+              </dgm:ruleLst>
+            </dgm:layoutNode>
+          </dgm:if>
+          <dgm:else name="Name13"/>
+        </dgm:choose>
+      </dgm:layoutNode>
+      <dgm:forEach name="Name14" axis="followSib" ptType="sibTrans" cnt="1">
+        <dgm:layoutNode name="sp">
+          <dgm:alg type="sp"/>
+          <dgm:shape xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:blip="">
+            <dgm:adjLst/>
+          </dgm:shape>
+          <dgm:presOf/>
+          <dgm:constrLst/>
+          <dgm:ruleLst/>
+        </dgm:layoutNode>
+      </dgm:forEach>
+    </dgm:forEach>
+  </dgm:layoutNode>
+</dgm:layoutDef>
+</file>
+
+<file path=xl/diagrams/quickStyle1.xml><?xml version="1.0" encoding="utf-8"?>
+<dgm:styleDef xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uniqueId="urn:microsoft.com/office/officeart/2005/8/quickstyle/simple4">
+  <dgm:title val=""/>
+  <dgm:desc val=""/>
+  <dgm:catLst>
+    <dgm:cat type="simple" pri="10400"/>
+  </dgm:catLst>
+  <dgm:scene3d>
+    <a:camera prst="orthographicFront"/>
+    <a:lightRig rig="threePt" dir="t"/>
+  </dgm:scene3d>
+  <dgm:styleLbl name="node0">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="3">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor">
+        <a:schemeClr val="lt1"/>
+      </a:fontRef>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="lnNode1">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="3">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor">
+        <a:schemeClr val="lt1"/>
+      </a:fontRef>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="vennNode1">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="3">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor">
+        <a:schemeClr val="tx1"/>
+      </a:fontRef>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="alignNode1">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="3">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor">
+        <a:schemeClr val="lt1"/>
+      </a:fontRef>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="node1">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="3">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor">
+        <a:schemeClr val="lt1"/>
+      </a:fontRef>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="node2">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="3">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor">
+        <a:schemeClr val="lt1"/>
+      </a:fontRef>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="node3">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="3">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor">
+        <a:schemeClr val="lt1"/>
+      </a:fontRef>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="node4">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="3">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor">
+        <a:schemeClr val="lt1"/>
+      </a:fontRef>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="fgImgPlace1">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor"/>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="alignImgPlace1">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor"/>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="bgImgPlace1">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor"/>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="sibTrans2D1">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="3">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor">
+        <a:schemeClr val="lt1"/>
+      </a:fontRef>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="fgSibTrans2D1">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="3">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor">
+        <a:schemeClr val="lt1"/>
+      </a:fontRef>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="bgSibTrans2D1">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="3">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor">
+        <a:schemeClr val="lt1"/>
+      </a:fontRef>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="sibTrans1D1">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor"/>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="callout">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor"/>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="asst0">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="3">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor">
+        <a:schemeClr val="lt1"/>
+      </a:fontRef>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="asst1">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="3">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor">
+        <a:schemeClr val="lt1"/>
+      </a:fontRef>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="asst2">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="3">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor">
+        <a:schemeClr val="lt1"/>
+      </a:fontRef>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="asst3">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="3">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor">
+        <a:schemeClr val="lt1"/>
+      </a:fontRef>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="asst4">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="3">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor">
+        <a:schemeClr val="lt1"/>
+      </a:fontRef>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="parChTrans2D1">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="3">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor">
+        <a:schemeClr val="lt1"/>
+      </a:fontRef>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="parChTrans2D2">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="3">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor">
+        <a:schemeClr val="lt1"/>
+      </a:fontRef>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="parChTrans2D3">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="3">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor">
+        <a:schemeClr val="lt1"/>
+      </a:fontRef>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="parChTrans2D4">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="3">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor">
+        <a:schemeClr val="lt1"/>
+      </a:fontRef>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="parChTrans1D1">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor"/>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="parChTrans1D2">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor"/>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="parChTrans1D3">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor"/>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="parChTrans1D4">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor"/>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="fgAcc1">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor"/>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="conFgAcc1">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor"/>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="alignAcc1">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor"/>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="trAlignAcc1">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor"/>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="bgAcc1">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor"/>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="solidFgAcc1">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor"/>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="solidAlignAcc1">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor"/>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="solidBgAcc1">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor"/>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="fgAccFollowNode1">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor"/>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="alignAccFollowNode1">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor"/>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="bgAccFollowNode1">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor"/>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="fgAcc0">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor"/>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="fgAcc2">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor"/>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="fgAcc3">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor"/>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="fgAcc4">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor"/>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="bgShp">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor"/>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="dkBgShp">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor"/>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="trBgShp">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor"/>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="fgShp">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="3">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor"/>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="revTx">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor"/>
+    </dgm:style>
+  </dgm:styleLbl>
+</dgm:styleDef>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>295275</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>628679</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>188714</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Diagram 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/diagram">
+          <dgm:relIds xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:dm="rId1" r:lo="rId2" r:qs="rId3" r:cs="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="8210550" cy="2114550"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Imagen 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="6448425" y="2781300"/>
+          <a:ext cx="8210550" cy="2114550"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -621,7 +3689,7 @@
         <xdr:cNvPr id="2" name="Imagen 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -653,83 +3721,85 @@
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
-      <sheetName val="Proyección"/>
+      <sheetName val="Proyección 2019-2020"/>
+      <sheetName val="Proyección 2019-2025"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0">
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1">
         <row r="4">
-          <cell r="D4">
-            <v>321800</v>
+          <cell r="I4">
+            <v>335144</v>
           </cell>
         </row>
         <row r="6">
-          <cell r="D6">
-            <v>131002</v>
+          <cell r="I6">
+            <v>129234</v>
           </cell>
         </row>
         <row r="9">
-          <cell r="D9">
-            <v>74645</v>
+          <cell r="I9">
+            <v>74176</v>
           </cell>
         </row>
         <row r="11">
-          <cell r="D11">
-            <v>264281</v>
+          <cell r="I11">
+            <v>277438</v>
           </cell>
         </row>
         <row r="12">
-          <cell r="D12">
-            <v>107785</v>
+          <cell r="I12">
+            <v>130067</v>
           </cell>
         </row>
         <row r="17">
-          <cell r="D17">
-            <v>62443</v>
+          <cell r="I17">
+            <v>63344</v>
           </cell>
         </row>
         <row r="18">
-          <cell r="D18">
-            <v>42297</v>
+          <cell r="I18">
+            <v>43125</v>
           </cell>
         </row>
         <row r="20">
-          <cell r="D20">
-            <v>63441</v>
+          <cell r="I20">
+            <v>66115</v>
           </cell>
         </row>
         <row r="22">
-          <cell r="D22">
-            <v>24688</v>
+          <cell r="I22">
+            <v>26378</v>
           </cell>
         </row>
         <row r="23">
-          <cell r="D23">
-            <v>26116</v>
+          <cell r="I23">
+            <v>26876</v>
           </cell>
         </row>
         <row r="24">
-          <cell r="D24">
-            <v>28439</v>
+          <cell r="I24">
+            <v>34375</v>
           </cell>
         </row>
         <row r="25">
-          <cell r="D25">
-            <v>24799</v>
+          <cell r="I25">
+            <v>25555</v>
           </cell>
         </row>
         <row r="31">
-          <cell r="D31">
-            <v>188821</v>
+          <cell r="I31">
+            <v>210917</v>
           </cell>
         </row>
         <row r="32">
-          <cell r="D32">
-            <v>117767</v>
+          <cell r="I32">
+            <v>127201</v>
           </cell>
         </row>
         <row r="33">
-          <cell r="D33">
-            <v>94590</v>
+          <cell r="I33">
+            <v>108372</v>
           </cell>
         </row>
       </sheetData>
@@ -1000,11 +4070,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N21"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O1" sqref="O1:O1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1024,45 +4094,45 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="G1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="H1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="I1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="J1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="K1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B2" s="5"/>
       <c r="C2" s="6">
@@ -1108,7 +4178,7 @@
     </row>
     <row r="3" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B3" s="13"/>
       <c r="C3" s="14">
@@ -1128,10 +4198,10 @@
     </row>
     <row r="4" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B4" s="20" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C4" s="14">
         <v>23253</v>
@@ -1179,10 +4249,10 @@
     </row>
     <row r="5" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="20" t="s">
         <v>16</v>
-      </c>
-      <c r="B5" s="20" t="s">
-        <v>18</v>
       </c>
       <c r="C5" s="14">
         <v>18486</v>
@@ -1230,10 +4300,10 @@
     </row>
     <row r="6" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B6" s="20" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C6" s="14">
         <v>71083</v>
@@ -1281,10 +4351,10 @@
     </row>
     <row r="7" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="15" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B7" s="20" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C7" s="14">
         <v>226477</v>
@@ -1332,10 +4402,10 @@
     </row>
     <row r="8" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B8" s="20" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C8" s="14">
         <v>70294</v>
@@ -1383,10 +4453,10 @@
     </row>
     <row r="9" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B9" s="20" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C9" s="14">
         <v>55128</v>
@@ -1434,10 +4504,10 @@
     </row>
     <row r="10" spans="1:14" s="24" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B10" s="22" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C10" s="14">
         <v>280029</v>
@@ -1485,10 +4555,10 @@
     </row>
     <row r="11" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="15" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B11" s="20" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C11" s="14">
         <v>20451</v>
@@ -1536,10 +4606,10 @@
     </row>
     <row r="12" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="15" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B12" s="20" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C12" s="14">
         <v>22025</v>
@@ -1587,10 +4657,10 @@
     </row>
     <row r="13" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="15" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B13" s="20" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C13" s="14">
         <v>57159</v>
@@ -1638,10 +4708,10 @@
     </row>
     <row r="14" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="15" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B14" s="20" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C14" s="14">
         <v>38341</v>
@@ -1689,10 +4759,10 @@
     </row>
     <row r="15" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="15" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B15" s="20" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C15" s="14">
         <v>126491</v>
@@ -1740,7 +4810,7 @@
     </row>
     <row r="16" spans="1:14" s="24" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="25" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B16" s="26"/>
       <c r="C16" s="14">
@@ -1760,10 +4830,10 @@
     </row>
     <row r="17" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="27" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B17" s="20" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C17" s="14">
         <v>95942</v>
@@ -1811,10 +4881,10 @@
     </row>
     <row r="18" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="B18" s="20" t="s">
         <v>29</v>
-      </c>
-      <c r="B18" s="20" t="s">
-        <v>31</v>
       </c>
       <c r="C18" s="14">
         <v>68675</v>
@@ -1862,10 +4932,10 @@
     </row>
     <row r="19" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="27" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B19" s="20" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C19" s="14">
         <v>144076</v>
@@ -1913,13 +4983,28 @@
     </row>
     <row r="21" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="L21" s="28" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="M21" s="29">
         <f>MAX(M4:M19)</f>
         <v>2880.0423502762392</v>
       </c>
       <c r="N21" s="29"/>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A22" s="39" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A23" s="39" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A24" s="39" t="s">
+        <v>58</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1927,11 +5012,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1952,45 +5037,45 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="G1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="H1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="I1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="J1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="K1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>11</v>
-      </c>
       <c r="M1" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B2" s="13"/>
       <c r="C2" s="14"/>
@@ -2008,14 +5093,14 @@
     </row>
     <row r="3" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B3" s="20" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C3" s="14">
-        <f>[1]Proyección!$D$23</f>
-        <v>26116</v>
+        <f>'[1]Proyección 2019-2025'!$I$23</f>
+        <v>26876</v>
       </c>
       <c r="D3" s="21">
         <v>0.61</v>
@@ -2031,43 +5116,43 @@
       </c>
       <c r="H3" s="18">
         <f>C3*D3</f>
-        <v>15930.76</v>
+        <v>16394.36</v>
       </c>
       <c r="I3" s="18">
         <f>H3*E3/100</f>
-        <v>2063.0334199999998</v>
+        <v>2123.0696199999998</v>
       </c>
       <c r="J3" s="18">
         <f>I3*F3/100</f>
-        <v>618.87102229016136</v>
+        <v>636.88074724576427</v>
       </c>
       <c r="K3" s="18">
         <f>((I3*G3)/100)</f>
-        <v>41.260668399999993</v>
+        <v>42.461392399999994</v>
       </c>
       <c r="L3" s="19">
         <f>(J3+K3)/C3</f>
-        <v>2.5276906520529996E-2</v>
+        <v>2.5276906520529999E-2</v>
       </c>
       <c r="M3" s="21">
         <f>(L3*C3*365)/1000</f>
-        <v>240.94806710190892</v>
+        <v>247.95988097070395</v>
       </c>
       <c r="N3" s="21">
         <f>M3/$M$20</f>
-        <v>7.2801703652250208E-2</v>
+        <v>6.5223147860820035E-2</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="20" t="s">
-        <v>18</v>
-      </c>
       <c r="C4" s="14">
-        <f>[1]Proyección!$D$24</f>
-        <v>28439</v>
+        <f>'[1]Proyección 2019-2025'!$I$24</f>
+        <v>34375</v>
       </c>
       <c r="D4" s="21">
         <v>0.61</v>
@@ -2083,19 +5168,19 @@
       </c>
       <c r="H4" s="18">
         <f>C4*D4</f>
-        <v>17347.79</v>
+        <v>20968.75</v>
       </c>
       <c r="I4" s="18">
         <f t="shared" ref="I4:J18" si="0">H4*E4/100</f>
-        <v>2246.5388049999997</v>
+        <v>2715.4531249999995</v>
       </c>
       <c r="J4" s="18">
         <f t="shared" si="0"/>
-        <v>673.9191684373526</v>
+        <v>814.58459914321861</v>
       </c>
       <c r="K4" s="18">
         <f t="shared" ref="K4:K18" si="1">((I4*G4)/100)</f>
-        <v>44.930776099999996</v>
+        <v>54.309062499999989</v>
       </c>
       <c r="L4" s="19">
         <f>(J4+K4)/C4</f>
@@ -2103,23 +5188,23 @@
       </c>
       <c r="M4" s="21">
         <f t="shared" ref="M4:M18" si="2">(L4*C4*365)/1000</f>
-        <v>262.3802297561337</v>
+        <v>317.14618649977479</v>
       </c>
       <c r="N4" s="21">
         <f t="shared" ref="N4:N18" si="3">M4/$M$20</f>
-        <v>7.9277364457280744E-2</v>
+        <v>8.3421852497235022E-2</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B5" s="20" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C5" s="14">
-        <f>[1]Proyección!$D$9</f>
-        <v>74645</v>
+        <f>'[1]Proyección 2019-2025'!$I$9</f>
+        <v>74176</v>
       </c>
       <c r="D5" s="21">
         <v>0.68</v>
@@ -2135,43 +5220,43 @@
       </c>
       <c r="H5" s="18">
         <f t="shared" ref="H5:H18" si="4">C5*D5</f>
-        <v>50758.600000000006</v>
+        <v>50439.68</v>
       </c>
       <c r="I5" s="18">
         <f t="shared" si="0"/>
-        <v>6573.2386999999999</v>
+        <v>6531.9385599999987</v>
       </c>
       <c r="J5" s="18">
         <f t="shared" si="0"/>
-        <v>1971.8473363491378</v>
+        <v>1959.4580751695842</v>
       </c>
       <c r="K5" s="18">
         <f t="shared" si="1"/>
-        <v>131.46477400000001</v>
+        <v>130.63877119999998</v>
       </c>
       <c r="L5" s="19">
         <f t="shared" ref="L5:L18" si="5">(J5+K5)/C5</f>
-        <v>2.8177535137639997E-2</v>
+        <v>2.817753513763999E-2</v>
       </c>
       <c r="M5" s="21">
         <f t="shared" si="2"/>
-        <v>767.70892027743525</v>
+        <v>762.88534892489815</v>
       </c>
       <c r="N5" s="21">
         <f t="shared" si="3"/>
-        <v>0.2319608452454941</v>
+        <v>0.2006686876884762</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B6" s="20" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C6" s="14">
-        <f>[1]Proyección!$D$11</f>
-        <v>264281</v>
+        <f>'[1]Proyección 2019-2025'!$I$11</f>
+        <v>277438</v>
       </c>
       <c r="D6" s="21">
         <v>0.68</v>
@@ -2187,43 +5272,43 @@
       </c>
       <c r="H6" s="18">
         <f t="shared" si="4"/>
-        <v>179711.08000000002</v>
+        <v>188657.84000000003</v>
       </c>
       <c r="I6" s="18">
         <f t="shared" si="0"/>
-        <v>23272.584859999995</v>
+        <v>24431.190279999999</v>
       </c>
       <c r="J6" s="18">
         <f t="shared" si="0"/>
-        <v>6981.3354665106363</v>
+        <v>7328.8951879165661</v>
       </c>
       <c r="K6" s="18">
         <f t="shared" si="1"/>
-        <v>465.4516971999999</v>
+        <v>488.62380559999997</v>
       </c>
       <c r="L6" s="19">
         <f t="shared" si="5"/>
-        <v>2.8177535137639997E-2</v>
+        <v>2.817753513764E-2</v>
       </c>
       <c r="M6" s="21">
         <f t="shared" si="2"/>
-        <v>2718.0773147543823</v>
+        <v>2853.3944326335468</v>
       </c>
       <c r="N6" s="21">
         <f t="shared" si="3"/>
-        <v>0.82125854568054701</v>
+        <v>0.7505543487774412</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="15" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B7" s="20" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C7" s="14">
-        <f>[1]Proyección!$D$12</f>
-        <v>107785</v>
+        <f>'[1]Proyección 2019-2025'!$I$12</f>
+        <v>130067</v>
       </c>
       <c r="D7" s="21">
         <v>0.68</v>
@@ -2239,43 +5324,43 @@
       </c>
       <c r="H7" s="18">
         <f t="shared" si="4"/>
-        <v>73293.8</v>
+        <v>88445.560000000012</v>
       </c>
       <c r="I7" s="18">
         <f t="shared" si="0"/>
-        <v>9491.547099999998</v>
+        <v>11453.700019999998</v>
       </c>
       <c r="J7" s="18">
         <f t="shared" si="0"/>
-        <v>2847.2846828105266</v>
+        <v>3435.8934623474215</v>
       </c>
       <c r="K7" s="18">
         <f t="shared" si="1"/>
-        <v>189.83094199999996</v>
+        <v>229.07400039999996</v>
       </c>
       <c r="L7" s="19">
         <f t="shared" si="5"/>
-        <v>2.8177535137639993E-2</v>
+        <v>2.8177535137639997E-2</v>
       </c>
       <c r="M7" s="21">
         <f t="shared" si="2"/>
-        <v>1108.5472030558424</v>
+        <v>1337.7131239028088</v>
       </c>
       <c r="N7" s="21">
         <f t="shared" si="3"/>
-        <v>0.33494406463642012</v>
+        <v>0.35187087739399586</v>
       </c>
     </row>
     <row r="8" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B8" s="20" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C8" s="14">
-        <f>[1]Proyección!$D$20</f>
-        <v>63441</v>
+        <f>'[1]Proyección 2019-2025'!$I$20</f>
+        <v>66115</v>
       </c>
       <c r="D8" s="21">
         <v>0.68</v>
@@ -2291,46 +5376,46 @@
       </c>
       <c r="H8" s="18">
         <f t="shared" si="4"/>
-        <v>43139.880000000005</v>
+        <v>44958.200000000004</v>
       </c>
       <c r="I8" s="18">
         <f t="shared" si="0"/>
-        <v>5586.6144599999998</v>
+        <v>5822.0868999999993</v>
       </c>
       <c r="J8" s="18">
         <f t="shared" si="0"/>
-        <v>1675.8787174670192</v>
+        <v>1746.5159976250684</v>
       </c>
       <c r="K8" s="18">
         <f t="shared" si="1"/>
-        <v>111.7322892</v>
+        <v>116.44173799999999</v>
       </c>
       <c r="L8" s="19">
         <f t="shared" si="5"/>
-        <v>2.817753513764E-2</v>
+        <v>2.8177535137639997E-2</v>
       </c>
       <c r="M8" s="21">
         <f t="shared" si="2"/>
-        <v>652.47801743346201</v>
+        <v>679.97957350314994</v>
       </c>
       <c r="N8" s="21">
         <f t="shared" si="3"/>
-        <v>0.1971441889372281</v>
+        <v>0.17886122582133851</v>
       </c>
     </row>
     <row r="9" spans="1:14" s="24" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B9" s="22" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C9" s="14">
-        <f>[1]Proyección!$D$4</f>
-        <v>321800</v>
+        <f>'[1]Proyección 2019-2025'!$I$4</f>
+        <v>335144</v>
       </c>
       <c r="D9" s="23">
-        <v>0.68</v>
+        <v>0.75</v>
       </c>
       <c r="E9" s="16">
         <v>12.949999999999998</v>
@@ -2343,27 +5428,27 @@
       </c>
       <c r="H9" s="18">
         <f t="shared" si="4"/>
-        <v>218824.00000000003</v>
+        <v>251358</v>
       </c>
       <c r="I9" s="18">
         <f t="shared" si="0"/>
-        <v>28337.707999999999</v>
+        <v>32550.86099999999</v>
       </c>
       <c r="J9" s="18">
         <f t="shared" si="0"/>
-        <v>8500.7766472925505</v>
+        <v>9764.6428934219311</v>
       </c>
       <c r="K9" s="18">
         <f t="shared" si="1"/>
-        <v>566.75415999999996</v>
+        <v>651.01721999999984</v>
       </c>
       <c r="L9" s="19">
         <f t="shared" si="5"/>
-        <v>2.8177535137639997E-2</v>
+        <v>3.1078163754749991E-2</v>
       </c>
       <c r="M9" s="21">
         <f t="shared" si="2"/>
-        <v>3309.6487446617812</v>
+        <v>3801.7159413990048</v>
       </c>
       <c r="N9" s="21">
         <f t="shared" si="3"/>
@@ -2372,14 +5457,14 @@
     </row>
     <row r="10" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B10" s="20" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C10" s="14">
-        <f>[1]Proyección!$D$22</f>
-        <v>24688</v>
+        <f>'[1]Proyección 2019-2025'!$I$22</f>
+        <v>26378</v>
       </c>
       <c r="D10" s="21">
         <v>0.61</v>
@@ -2395,43 +5480,43 @@
       </c>
       <c r="H10" s="18">
         <f t="shared" si="4"/>
-        <v>15059.68</v>
+        <v>16090.58</v>
       </c>
       <c r="I10" s="18">
         <f t="shared" si="0"/>
-        <v>1950.2285599999998</v>
+        <v>2083.7301099999995</v>
       </c>
       <c r="J10" s="18">
         <f t="shared" si="0"/>
-        <v>585.03169697884459</v>
+        <v>625.07963799854019</v>
       </c>
       <c r="K10" s="18">
         <f t="shared" si="1"/>
-        <v>39.004571199999994</v>
+        <v>41.674602199999988</v>
       </c>
       <c r="L10" s="19">
         <f t="shared" si="5"/>
-        <v>2.5276906520529996E-2</v>
+        <v>2.5276906520529992E-2</v>
       </c>
       <c r="M10" s="21">
         <f t="shared" si="2"/>
-        <v>227.77323788527826</v>
+        <v>243.36529767246716</v>
       </c>
       <c r="N10" s="21">
         <f t="shared" si="3"/>
-        <v>6.8820970277483268E-2</v>
+        <v>6.4014592732278261E-2</v>
       </c>
     </row>
     <row r="11" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="15" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B11" s="20" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C11" s="14">
-        <f>[1]Proyección!$D$25</f>
-        <v>24799</v>
+        <f>'[1]Proyección 2019-2025'!$I$25</f>
+        <v>25555</v>
       </c>
       <c r="D11" s="21">
         <v>0.61</v>
@@ -2447,43 +5532,43 @@
       </c>
       <c r="H11" s="18">
         <f t="shared" si="4"/>
-        <v>15127.39</v>
+        <v>15588.55</v>
       </c>
       <c r="I11" s="18">
         <f t="shared" si="0"/>
-        <v>1958.9970049999995</v>
+        <v>2018.7172249999994</v>
       </c>
       <c r="J11" s="18">
         <f t="shared" si="0"/>
-        <v>587.6620647026233</v>
+        <v>605.57700163214406</v>
       </c>
       <c r="K11" s="18">
         <f t="shared" si="1"/>
-        <v>39.179940099999989</v>
+        <v>40.374344499999985</v>
       </c>
       <c r="L11" s="19">
         <f t="shared" si="5"/>
-        <v>2.5276906520529992E-2</v>
+        <v>2.5276906520529996E-2</v>
       </c>
       <c r="M11" s="21">
         <f t="shared" si="2"/>
-        <v>228.79733175295749</v>
+        <v>235.77224133823259</v>
       </c>
       <c r="N11" s="21">
         <f t="shared" si="3"/>
-        <v>6.9130397031404223E-2</v>
+        <v>6.2017321907399017E-2</v>
       </c>
     </row>
     <row r="12" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="15" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B12" s="20" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C12" s="14">
-        <f>[1]Proyección!$D$17</f>
-        <v>62443</v>
+        <f>'[1]Proyección 2019-2025'!$I$17</f>
+        <v>63344</v>
       </c>
       <c r="D12" s="21">
         <v>0.68</v>
@@ -2499,43 +5584,43 @@
       </c>
       <c r="H12" s="18">
         <f t="shared" si="4"/>
-        <v>42461.240000000005</v>
+        <v>43073.920000000006</v>
       </c>
       <c r="I12" s="18">
         <f t="shared" si="0"/>
-        <v>5498.7305799999995</v>
+        <v>5578.0726399999994</v>
       </c>
       <c r="J12" s="18">
         <f t="shared" si="0"/>
-        <v>1649.5152149996543</v>
+        <v>1673.316332958668</v>
       </c>
       <c r="K12" s="18">
         <f t="shared" si="1"/>
-        <v>109.97461159999999</v>
+        <v>111.56145279999998</v>
       </c>
       <c r="L12" s="19">
         <f t="shared" si="5"/>
-        <v>2.8177535137639993E-2</v>
+        <v>2.8177535137639997E-2</v>
       </c>
       <c r="M12" s="21">
         <f t="shared" si="2"/>
-        <v>642.21378670887384</v>
+        <v>651.4803918019137</v>
       </c>
       <c r="N12" s="21">
         <f t="shared" si="3"/>
-        <v>0.19404288377874457</v>
+        <v>0.17136482626373539</v>
       </c>
     </row>
     <row r="13" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="15" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B13" s="20" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C13" s="14">
-        <f>[1]Proyección!$D$18</f>
-        <v>42297</v>
+        <f>'[1]Proyección 2019-2025'!$I$18</f>
+        <v>43125</v>
       </c>
       <c r="D13" s="21">
         <v>0.61</v>
@@ -2551,43 +5636,43 @@
       </c>
       <c r="H13" s="18">
         <f t="shared" si="4"/>
-        <v>25801.17</v>
+        <v>26306.25</v>
       </c>
       <c r="I13" s="18">
         <f t="shared" si="0"/>
-        <v>3341.251514999999</v>
+        <v>3406.6593749999993</v>
       </c>
       <c r="J13" s="18">
         <f t="shared" si="0"/>
-        <v>1002.3122847988571</v>
+        <v>1021.9334061978561</v>
       </c>
       <c r="K13" s="18">
         <f t="shared" si="1"/>
-        <v>66.82503029999998</v>
+        <v>68.133187499999991</v>
       </c>
       <c r="L13" s="19">
         <f t="shared" si="5"/>
-        <v>2.5276906520529992E-2</v>
+        <v>2.5276906520529999E-2</v>
       </c>
       <c r="M13" s="21">
         <f t="shared" si="2"/>
-        <v>390.23512001108281</v>
+        <v>397.87430669971752</v>
       </c>
       <c r="N13" s="21">
         <f t="shared" si="3"/>
-        <v>0.11790831901436769</v>
+        <v>0.1046565058601676</v>
       </c>
     </row>
     <row r="14" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="15" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B14" s="20" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C14" s="14">
-        <f>[1]Proyección!$D$6</f>
-        <v>131002</v>
+        <f>'[1]Proyección 2019-2025'!$I$6</f>
+        <v>129234</v>
       </c>
       <c r="D14" s="21">
         <v>0.68</v>
@@ -2603,36 +5688,36 @@
       </c>
       <c r="H14" s="18">
         <f t="shared" si="4"/>
-        <v>89081.36</v>
+        <v>87879.12000000001</v>
       </c>
       <c r="I14" s="18">
         <f t="shared" si="0"/>
-        <v>11536.036119999997</v>
+        <v>11380.346039999999</v>
       </c>
       <c r="J14" s="18">
         <f t="shared" si="0"/>
-        <v>3460.5927357011142</v>
+        <v>3413.8886551777673</v>
       </c>
       <c r="K14" s="18">
         <f t="shared" si="1"/>
-        <v>230.72072239999994</v>
+        <v>227.60692079999998</v>
       </c>
       <c r="L14" s="19">
         <f t="shared" si="5"/>
-        <v>2.817753513763999E-2</v>
+        <v>2.8177535137639997E-2</v>
       </c>
       <c r="M14" s="21">
         <f t="shared" si="2"/>
-        <v>1347.3294122069067</v>
+        <v>1329.1458852318851</v>
       </c>
       <c r="N14" s="21">
         <f t="shared" si="3"/>
-        <v>0.40709136109384703</v>
+        <v>0.34961735850858144</v>
       </c>
     </row>
     <row r="15" spans="1:14" s="24" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="25" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B15" s="26"/>
       <c r="C15" s="14"/>
@@ -2650,14 +5735,14 @@
     </row>
     <row r="16" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="27" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B16" s="20" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C16" s="14">
-        <f>[1]Proyección!$D$32</f>
-        <v>117767</v>
+        <f>'[1]Proyección 2019-2025'!$I$32</f>
+        <v>127201</v>
       </c>
       <c r="D16" s="21">
         <v>0.68</v>
@@ -2673,43 +5758,43 @@
       </c>
       <c r="H16" s="18">
         <f t="shared" si="4"/>
-        <v>80081.560000000012</v>
+        <v>86496.680000000008</v>
       </c>
       <c r="I16" s="18">
         <f t="shared" si="0"/>
-        <v>10370.562019999999</v>
+        <v>11201.320059999998</v>
       </c>
       <c r="J16" s="18">
         <f t="shared" si="0"/>
-        <v>3110.9725401544497</v>
+        <v>3360.1842458429451</v>
       </c>
       <c r="K16" s="18">
         <f t="shared" si="1"/>
-        <v>207.4112404</v>
+        <v>224.02640119999995</v>
       </c>
       <c r="L16" s="19">
         <f t="shared" si="5"/>
-        <v>2.817753513764E-2</v>
+        <v>2.8177535137639993E-2</v>
       </c>
       <c r="M16" s="21">
         <f t="shared" si="2"/>
-        <v>1211.2100799023742</v>
+        <v>1308.2368861706748</v>
       </c>
       <c r="N16" s="21">
         <f t="shared" si="3"/>
-        <v>0.36596333126165326</v>
+        <v>0.34411747388187364</v>
       </c>
     </row>
     <row r="17" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="B17" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="B17" s="20" t="s">
-        <v>31</v>
-      </c>
       <c r="C17" s="14">
-        <f>[1]Proyección!$D$33</f>
-        <v>94590</v>
+        <f>'[1]Proyección 2019-2025'!$I$33</f>
+        <v>108372</v>
       </c>
       <c r="D17" s="21">
         <v>0.68</v>
@@ -2725,43 +5810,43 @@
       </c>
       <c r="H17" s="18">
         <f t="shared" si="4"/>
-        <v>64321.200000000004</v>
+        <v>73692.960000000006</v>
       </c>
       <c r="I17" s="18">
         <f t="shared" si="0"/>
-        <v>8329.5953999999983</v>
+        <v>9543.2383199999986</v>
       </c>
       <c r="J17" s="18">
         <f t="shared" si="0"/>
-        <v>2498.7211406693673</v>
+        <v>2862.7910715363214</v>
       </c>
       <c r="K17" s="18">
         <f t="shared" si="1"/>
-        <v>166.59190799999996</v>
+        <v>190.86476639999998</v>
       </c>
       <c r="L17" s="19">
         <f t="shared" si="5"/>
-        <v>2.8177535137639997E-2</v>
+        <v>2.8177535137639993E-2</v>
       </c>
       <c r="M17" s="21">
         <f t="shared" si="2"/>
-        <v>972.83926276431896</v>
+        <v>1114.5843808467573</v>
       </c>
       <c r="N17" s="21">
         <f t="shared" si="3"/>
-        <v>0.29394033561218147</v>
+        <v>0.29317929009619748</v>
       </c>
     </row>
     <row r="18" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="27" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B18" s="20" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C18" s="14">
-        <f>[1]Proyección!$D$31</f>
-        <v>188821</v>
+        <f>'[1]Proyección 2019-2025'!$I$31</f>
+        <v>210917</v>
       </c>
       <c r="D18" s="21">
         <v>0.68</v>
@@ -2777,60 +5862,73 @@
       </c>
       <c r="H18" s="18">
         <f t="shared" si="4"/>
-        <v>128398.28000000001</v>
+        <v>143423.56</v>
       </c>
       <c r="I18" s="18">
         <f t="shared" si="0"/>
-        <v>16627.577259999998</v>
+        <v>18573.351019999998</v>
       </c>
       <c r="J18" s="18">
         <f t="shared" si="0"/>
-        <v>4987.9588170243214</v>
+        <v>5571.6541582256159</v>
       </c>
       <c r="K18" s="18">
         <f t="shared" si="1"/>
-        <v>332.55154519999996</v>
+        <v>371.46702039999997</v>
       </c>
       <c r="L18" s="19">
         <f t="shared" si="5"/>
-        <v>2.8177535137639993E-2</v>
+        <v>2.817753513764E-2</v>
       </c>
       <c r="M18" s="21">
         <f t="shared" si="2"/>
-        <v>1941.9862822118773</v>
+        <v>2169.23923019835</v>
       </c>
       <c r="N18" s="21">
         <f t="shared" si="3"/>
-        <v>0.58676507147296453</v>
+        <v>0.57059476921363173</v>
       </c>
     </row>
     <row r="20" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="L20" s="28" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="M20" s="29">
         <f>MAX(M3:M18)</f>
-        <v>3309.6487446617812</v>
+        <v>3801.7159413990048</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A21" s="39" t="s">
+        <v>52</v>
+      </c>
       <c r="N21" s="29"/>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A22" s="39" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A23" s="39" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B27" s="15"/>
       <c r="C27" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="D27" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="E27" s="15" t="s">
         <v>33</v>
-      </c>
-      <c r="D27" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="E27" s="15" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B28" s="15" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C28" s="30">
         <v>0</v>
@@ -2844,7 +5942,7 @@
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B29" s="15" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C29" s="30">
         <v>15001</v>
@@ -2858,7 +5956,7 @@
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B30" s="15" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C30" s="30">
         <v>50001</v>
@@ -2872,7 +5970,7 @@
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B31" s="15" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C31" s="30">
         <v>300001</v>
@@ -2886,13 +5984,13 @@
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B32" s="15" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C32" s="30">
         <v>500001</v>
       </c>
       <c r="D32" s="30" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E32" s="30">
         <v>0.98</v>
@@ -2904,11 +6002,120 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C2:F8"/>
+  <sheetViews>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16" customWidth="1"/>
+    <col min="5" max="5" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C2" s="15"/>
+      <c r="D2" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="E2" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="F2" s="15" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C3" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3" s="30">
+        <v>0</v>
+      </c>
+      <c r="E3" s="30">
+        <v>15000</v>
+      </c>
+      <c r="F3" s="30">
+        <v>0.56000000000000005</v>
+      </c>
+    </row>
+    <row r="4" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C4" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="D4" s="30">
+        <v>15001</v>
+      </c>
+      <c r="E4" s="30">
+        <v>50000</v>
+      </c>
+      <c r="F4" s="30">
+        <v>0.61</v>
+      </c>
+    </row>
+    <row r="5" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C5" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="D5" s="30">
+        <v>50001</v>
+      </c>
+      <c r="E5" s="30">
+        <v>300000</v>
+      </c>
+      <c r="F5" s="30">
+        <v>0.68</v>
+      </c>
+    </row>
+    <row r="6" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C6" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="D6" s="30">
+        <v>300001</v>
+      </c>
+      <c r="E6" s="30">
+        <v>500000</v>
+      </c>
+      <c r="F6" s="30">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="7" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C7" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="D7" s="30">
+        <v>500001</v>
+      </c>
+      <c r="E7" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="F7" s="30">
+        <v>0.98</v>
+      </c>
+    </row>
+    <row r="8" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="D8" s="40"/>
+      <c r="E8" s="40"/>
+      <c r="F8" s="40"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2919,37 +6126,37 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="15"/>
-      <c r="B1" s="38" t="s">
-        <v>48</v>
-      </c>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
+      <c r="B1" s="41" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
       <c r="E1" s="36" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:5" s="31" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="36"/>
       <c r="B2" s="37" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" s="37" t="s">
+        <v>42</v>
+      </c>
+      <c r="D2" s="37" t="s">
         <v>47</v>
       </c>
-      <c r="C2" s="37" t="s">
-        <v>44</v>
-      </c>
-      <c r="D2" s="37" t="s">
-        <v>49</v>
-      </c>
       <c r="E2" s="37" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="32" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B3" s="33">
-        <f>MEDIAN('trash 2020'!N3:N14)</f>
-        <v>0.19559353635798632</v>
+        <f>MEDIAN('trash 2025'!N3:N14)</f>
+        <v>0.17511302604253695</v>
       </c>
       <c r="C3" s="33">
         <f>MEDIAN('trash 2010'!N4:N15)</f>
@@ -2957,20 +6164,20 @@
       </c>
       <c r="D3" s="32">
         <f>(B3-C3)/C3</f>
-        <v>-2.443092445624977E-2</v>
+        <v>-0.12658231906337206</v>
       </c>
       <c r="E3" s="32">
         <f>D3/10</f>
-        <v>-2.443092445624977E-3</v>
+        <v>-1.2658231906337206E-2</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="34" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B4" s="35">
-        <f>MEDIAN('trash 2020'!N16:N18)</f>
-        <v>0.36596333126165326</v>
+        <f>MEDIAN('trash 2025'!N16:N18)</f>
+        <v>0.34411747388187364</v>
       </c>
       <c r="C4" s="35">
         <f>MEDIAN('trash 2010'!N17:N19)</f>
@@ -2978,11 +6185,11 @@
       </c>
       <c r="D4" s="34">
         <f>(B4-C4)/C4</f>
-        <v>6.8148940921280626E-2</v>
+        <v>4.3867346278709867E-3</v>
       </c>
       <c r="E4" s="34">
         <f>D4/10</f>
-        <v>6.8148940921280623E-3</v>
+        <v>4.3867346278709867E-4</v>
       </c>
     </row>
   </sheetData>
@@ -2994,25 +6201,25 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B9742B7-56DA-4CF7-B852-0045A1AE0776}">
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="39" t="s">
-        <v>52</v>
-      </c>
-      <c r="B1" s="39" t="s">
-        <v>53</v>
-      </c>
-      <c r="C1" s="39" t="s">
-        <v>54</v>
+      <c r="A1" s="38" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" s="38" t="s">
+        <v>50</v>
+      </c>
+      <c r="C1" s="38" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -3024,7 +6231,7 @@
       </c>
       <c r="C2">
         <f>'calculo trash'!E4</f>
-        <v>6.8148940921280623E-3</v>
+        <v>4.3867346278709867E-4</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -3036,7 +6243,7 @@
       </c>
       <c r="C3">
         <f>'calculo trash'!E3</f>
-        <v>-2.443092445624977E-3</v>
+        <v>-1.2658231906337206E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>